<commit_message>
switching to seq, still need to map class and pgm
</commit_message>
<xml_diff>
--- a/sql/nclass.xlsx
+++ b/sql/nclass.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="56">
   <si>
     <t>Adult</t>
   </si>
@@ -142,13 +142,58 @@
   </si>
   <si>
     <t>wellness</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>Adult ATP</t>
+  </si>
+  <si>
+    <t>Adult Basic</t>
+  </si>
+  <si>
+    <t>Adult Single Class</t>
+  </si>
+  <si>
+    <t>Adult Unlimited</t>
+  </si>
+  <si>
+    <t>BBT</t>
+  </si>
+  <si>
+    <t>Children Basic</t>
+  </si>
+  <si>
+    <t>Children Single BBT</t>
+  </si>
+  <si>
+    <t>Children Single Class</t>
+  </si>
+  <si>
+    <t>Children Single Ldr</t>
+  </si>
+  <si>
+    <t>Intro Karate</t>
+  </si>
+  <si>
+    <t>Leadership</t>
+  </si>
+  <si>
+    <t>Tai Chi Drop In</t>
+  </si>
+  <si>
+    <t>nclasslist</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -283,8 +328,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -464,8 +522,20 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE5E5E5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -580,6 +650,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -625,8 +710,17 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -948,15 +1042,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H22"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="108.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1495,7 +1591,285 @@
         <v>update nclasspays set classseq = 21 where class = 'Zoomba';</v>
       </c>
     </row>
+    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>1</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H26" t="str">
+        <f>"update nclasspays set pgmseq = " &amp; A26 &amp; " where classid = '" &amp; B26 &amp; "';"</f>
+        <v>update nclasspays set pgmseq = 1 where classid = 'Adult ATP';</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>2</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H27" t="str">
+        <f t="shared" ref="H27:H47" si="2">"update nclasspays set pgmseq = " &amp; A27 &amp; " where classid = '" &amp; B27 &amp; "';"</f>
+        <v>update nclasspays set pgmseq = 2 where classid = 'Adult Basic';</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <v>3</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H28" t="str">
+        <f t="shared" si="2"/>
+        <v>update nclasspays set pgmseq = 3 where classid = 'Adult Single Class';</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>4</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H29" t="str">
+        <f t="shared" si="2"/>
+        <v>update nclasspays set pgmseq = 4 where classid = 'Adult Unlimited';</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <v>5</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H30" t="str">
+        <f t="shared" si="2"/>
+        <v>update nclasspays set pgmseq = 5 where classid = 'After School';</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
+        <v>6</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H31" t="str">
+        <f t="shared" si="2"/>
+        <v>update nclasspays set pgmseq = 6 where classid = 'BBT';</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
+        <v>7</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H32" t="str">
+        <f t="shared" si="2"/>
+        <v>update nclasspays set pgmseq = 7 where classid = 'Blackbelt Adult';</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
+        <v>8</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H33" t="str">
+        <f t="shared" si="2"/>
+        <v>update nclasspays set pgmseq = 8 where classid = 'Blackbelt Jr';</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
+        <v>9</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H34" t="str">
+        <f t="shared" si="2"/>
+        <v>update nclasspays set pgmseq = 9 where classid = 'Children Basic';</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="2">
+        <v>10</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H35" t="str">
+        <f t="shared" si="2"/>
+        <v>update nclasspays set pgmseq = 10 where classid = 'Children Single BBT';</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="2">
+        <v>11</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H36" t="str">
+        <f t="shared" si="2"/>
+        <v>update nclasspays set pgmseq = 11 where classid = 'Children Single Class';</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
+        <v>12</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H37" t="str">
+        <f t="shared" si="2"/>
+        <v>update nclasspays set pgmseq = 12 where classid = 'Children Single Ldr';</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="2">
+        <v>13</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H38" t="str">
+        <f t="shared" si="2"/>
+        <v>update nclasspays set pgmseq = 13 where classid = 'Intro Karate';</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="2">
+        <v>14</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H39" t="str">
+        <f t="shared" si="2"/>
+        <v>update nclasspays set pgmseq = 14 where classid = 'Kickboxing';</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="2">
+        <v>15</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H40" t="str">
+        <f t="shared" si="2"/>
+        <v>update nclasspays set pgmseq = 15 where classid = 'Leadership';</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="2">
+        <v>16</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H41" t="str">
+        <f t="shared" si="2"/>
+        <v>update nclasspays set pgmseq = 16 where classid = 'Privates Adult';</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="2">
+        <v>17</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H42" t="str">
+        <f t="shared" si="2"/>
+        <v>update nclasspays set pgmseq = 17 where classid = 'Privates Children';</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="2">
+        <v>18</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H43" t="str">
+        <f t="shared" si="2"/>
+        <v>update nclasspays set pgmseq = 18 where classid = 'Self Defense';</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="2">
+        <v>19</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H44" t="str">
+        <f t="shared" si="2"/>
+        <v>update nclasspays set pgmseq = 19 where classid = 'Special Needs';</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="2">
+        <v>20</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H45" t="str">
+        <f t="shared" si="2"/>
+        <v>update nclasspays set pgmseq = 20 where classid = 'Tai Chi Drop In';</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="2">
+        <v>21</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H46" t="str">
+        <f t="shared" si="2"/>
+        <v>update nclasspays set pgmseq = 21 where classid = 'TaiChi';</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="2">
+        <v>22</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H47" t="str">
+        <f t="shared" si="2"/>
+        <v>update nclasspays set pgmseq = 22 where classid = 'Zoomba';</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>